<commit_message>
Add MTZ constraints to avoid loops
</commit_message>
<xml_diff>
--- a/data/37-intersection map Solution.xlsx
+++ b/data/37-intersection map Solution.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -615,6 +615,96 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>25</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>27</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>29</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>30</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>31</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>38</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -627,7 +717,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -657,7 +747,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -665,10 +755,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -676,10 +766,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -687,10 +777,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="n">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -698,10 +788,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -709,10 +799,10 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -720,10 +810,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -731,12 +821,78 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>19</v>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>20</v>
+      </c>
+      <c r="B12" t="n">
+        <v>19</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>27</v>
+      </c>
+      <c r="B13" t="n">
+        <v>25</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>30</v>
       </c>
-      <c r="C9" t="n">
+      <c r="B14" t="n">
+        <v>29</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>31</v>
+      </c>
+      <c r="B15" t="n">
+        <v>30</v>
+      </c>
+      <c r="C15" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>